<commit_message>
progression analysis complex query
</commit_message>
<xml_diff>
--- a/analysis/interpretation/analysis query/sumary_table.xlsx
+++ b/analysis/interpretation/analysis query/sumary_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="definition" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">is rejected by intersection</t>
   </si>
@@ -65,28 +65,43 @@
     <t xml:space="preserve">yes, with LDES and intersection hypothesis</t>
   </si>
   <si>
+    <t>Variante</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
     <t>Query</t>
   </si>
   <si>
-    <t>Post</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
     <t xml:space="preserve">Can traverse a subset</t>
   </si>
   <si>
+    <t>V1</t>
+  </si>
+  <si>
     <t>Q1</t>
   </si>
   <si>
+    <t>V2</t>
+  </si>
+  <si>
     <t>Q2</t>
   </si>
   <si>
+    <t>V3</t>
+  </si>
+  <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>V4</t>
   </si>
   <si>
     <t>Q4</t>
@@ -162,23 +177,17 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,7 +713,7 @@
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="D6" s="1" t="s">
@@ -713,44 +722,44 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="I7" s="4" t="s">
+      <c r="F7" s="1"/>
+      <c r="I7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="8" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" t="s">
         <v>11</v>
       </c>
@@ -759,15 +768,15 @@
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="6" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -795,27 +804,30 @@
   <cols>
     <col bestFit="1" min="5" max="5" width="22.57421875"/>
     <col bestFit="1" min="6" max="6" width="19.00390625"/>
-    <col bestFit="1" min="11" max="11" width="16.140625"/>
+    <col bestFit="1" min="11" max="11" width="9.140625"/>
     <col bestFit="1" min="14" max="14" width="20.57421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="J1"/>
-      <c r="K1" s="9"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -827,17 +839,16 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
+        <v>21</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" t="str">
         <f>definition!D7</f>
@@ -847,49 +858,45 @@
         <f>definition!D7</f>
         <v>weak</v>
       </c>
-      <c r="E4" s="7" t="str">
+      <c r="E4" s="4" t="str">
         <f>definition!D8</f>
         <v>strong</v>
       </c>
-      <c r="F4" s="11" t="str">
+      <c r="F4" s="5" t="str">
         <f>definition!I8</f>
         <v xml:space="preserve">yes, with LDSE test</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="11" t="str">
-        <f>definition!D7</f>
-        <v>weak</v>
-      </c>
-      <c r="D5" s="11" t="str">
-        <f>definition!D7</f>
-        <v>weak</v>
-      </c>
-      <c r="E5" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>definition!D7</f>
+        <v>weak</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f>definition!D7</f>
+        <v>weak</v>
+      </c>
+      <c r="E5" s="4" t="str">
         <f>definition!D8</f>
         <v>strong</v>
       </c>
-      <c r="F5" s="5" t="str">
+      <c r="F5" s="3" t="str">
         <f>definition!I7</f>
         <v>no</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" t="str">
         <f>definition!D7</f>
@@ -907,10 +914,13 @@
         <f>definition!I7</f>
         <v>no</v>
       </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C7" t="str">
         <f>definition!D7</f>
@@ -931,7 +941,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="B8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" t="str">
         <f>definition!D7</f>
@@ -952,7 +962,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C9" t="str">
         <f>definition!D8</f>
@@ -973,7 +983,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C10" t="str">
         <f>definition!D7</f>
@@ -1007,9 +1017,9 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="6" max="6" width="22.57421875"/>
+    <col customWidth="1" min="6" max="6" width="25.140625"/>
     <col bestFit="1" min="7" max="7" width="37.00390625"/>
   </cols>
   <sheetData>
@@ -1037,7 +1047,7 @@
     </row>
     <row r="4">
       <c r="C4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" t="str">
         <f>definition!D8</f>
@@ -1057,8 +1067,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="9" t="s">
-        <v>22</v>
+      <c r="C5" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="D5" t="str">
         <f>definition!D8</f>
@@ -1078,8 +1088,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="9" t="s">
-        <v>23</v>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D6" t="str">
         <f>definition!D7</f>
@@ -1098,12 +1108,12 @@
         <v>no</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
-      <c r="C7" s="9" t="s">
-        <v>24</v>
+      <c r="C7" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D7" t="str">
         <f>definition!D7</f>
@@ -1123,8 +1133,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="9" t="s">
-        <v>25</v>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D8" t="str">
         <f>definition!D7</f>
@@ -1144,8 +1154,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="9" t="s">
-        <v>26</v>
+      <c r="C9" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D9" t="str">
         <f>definition!D7</f>
@@ -1165,8 +1175,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="9" t="s">
-        <v>27</v>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D10" t="str">
         <f>definition!D7</f>
@@ -1186,8 +1196,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="9" t="s">
-        <v>29</v>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D11" t="str">
         <f>definition!D7</f>

</xml_diff>